<commit_message>
Improves implementation of external scenarios
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-syngas.xlsx
+++ b/premise/data/additional_inventories/lci-syngas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467AA586-EB61-CD42-92B2-6EB10E4E0587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C17057-12A8-9540-8C67-F24862A33F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Syngas" sheetId="1" r:id="rId1"/>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>